<commit_message>
PSHCDT-93 :ERM Content Updates Based on Demo
</commit_message>
<xml_diff>
--- a/app/data/pool_index.xlsx
+++ b/app/data/pool_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\discovery\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60A6759-A789-4E7C-A4F9-3EFB622C1197}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760CF9DC-92D5-471D-922D-3A4624D72430}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4024" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4025" uniqueCount="1054">
   <si>
     <t>number</t>
   </si>
@@ -3109,9 +3109,6 @@
     <t>Tier 2</t>
   </si>
   <si>
-    <t>schedule36@gsa.gov</t>
-  </si>
-  <si>
     <t>https://www.gsa.gov/buying-selling/purchasing-programs/gsa-schedules/list-of-gsa-schedules/schedule-36imaging-document-solution/records-management-solutions</t>
   </si>
   <si>
@@ -3191,6 +3188,12 @@
   </si>
   <si>
     <t>HCATS Pool 2</t>
+  </si>
+  <si>
+    <t>R617</t>
+  </si>
+  <si>
+    <t>RecordsManagement@gsa.gov</t>
   </si>
 </sst>
 </file>
@@ -3686,9 +3689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3884,19 +3887,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1027</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1028</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>1025</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1026</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
@@ -3916,7 +3919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMI71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
@@ -4429,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>50</v>
@@ -4443,7 +4446,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -4752,123 +4755,123 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B62" s="1">
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B63" s="1">
         <v>3</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B64" s="1">
         <v>4</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B65" s="1">
         <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B66" s="1">
         <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B67" s="1">
         <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B68" s="1">
         <v>8</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B69" s="1">
         <v>9</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B70" s="1">
         <v>10</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B71" s="1">
         <v>11</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>
@@ -5081,37 +5084,37 @@
         <v>146</v>
       </c>
       <c r="BI1" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>1047</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>1049</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="2" spans="1:71" x14ac:dyDescent="0.2">
@@ -6879,13 +6882,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMK881"/>
+  <dimension ref="A1:AMK882"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B822" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BH825" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A710" sqref="A710"/>
-      <selection pane="bottomRight" activeCell="D848" sqref="D848"/>
+      <selection pane="bottomRight" activeCell="BI832" sqref="BI832:BS832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7075,37 +7078,37 @@
         <v>146</v>
       </c>
       <c r="BI1" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>1047</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>1048</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>1049</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="2" spans="1:71" x14ac:dyDescent="0.2">
@@ -17321,7 +17324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="817" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A817" s="1" t="s">
         <v>923</v>
       </c>
@@ -17344,7 +17347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="818" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="818" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A818" s="1" t="s">
         <v>924</v>
       </c>
@@ -17355,7 +17358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="819" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="819" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A819" s="1" t="s">
         <v>925</v>
       </c>
@@ -17366,7 +17369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="820" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="820" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A820" s="1" t="s">
         <v>926</v>
       </c>
@@ -17377,7 +17380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="821" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A821" s="1" t="s">
         <v>927</v>
       </c>
@@ -17388,7 +17391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="822" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="822" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A822" s="1" t="s">
         <v>928</v>
       </c>
@@ -17399,7 +17402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="823" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="823" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A823" s="1" t="s">
         <v>929</v>
       </c>
@@ -17410,7 +17413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="824" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="824" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A824" s="1" t="s">
         <v>930</v>
       </c>
@@ -17424,7 +17427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="825" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="825" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A825" s="1" t="s">
         <v>931</v>
       </c>
@@ -17435,7 +17438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="826" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="826" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A826" s="1" t="s">
         <v>932</v>
       </c>
@@ -17446,7 +17449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="827" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="827" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A827" s="1" t="s">
         <v>933</v>
       </c>
@@ -17457,7 +17460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="828" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="828" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A828" s="1" t="s">
         <v>934</v>
       </c>
@@ -17468,7 +17471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="829" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A829" s="1" t="s">
         <v>935</v>
       </c>
@@ -17479,7 +17482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="830" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="830" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A830" s="1" t="s">
         <v>936</v>
       </c>
@@ -17490,7 +17493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="831" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="831" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A831" s="1" t="s">
         <v>937</v>
       </c>
@@ -17501,26 +17504,47 @@
         <v>16</v>
       </c>
     </row>
-    <row r="832" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="832" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A832" s="1" t="s">
-        <v>938</v>
-      </c>
-      <c r="B832" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C832" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R832" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S832" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="BI832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BM832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BO832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BP832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BQ832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR832" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="BS832" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="833" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A833" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B833" s="1" t="s">
         <v>16</v>
@@ -17528,13 +17552,16 @@
       <c r="C833" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V833" s="1" t="s">
+      <c r="R833" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S833" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="834" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A834" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B834" s="1" t="s">
         <v>16</v>
@@ -17542,30 +17569,30 @@
       <c r="C834" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R834" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S834" s="1" t="s">
+      <c r="V834" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="835" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A835" s="1" t="s">
-        <v>941</v>
-      </c>
-      <c r="D835" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E835" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U835" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B835" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C835" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R835" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S835" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="836" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A836" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -17579,7 +17606,7 @@
     </row>
     <row r="837" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A837" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -17593,21 +17620,21 @@
     </row>
     <row r="838" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A838" s="1" t="s">
-        <v>944</v>
-      </c>
-      <c r="B838" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C838" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X838" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D838" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E838" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U838" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="839" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A839" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B839" s="1" t="s">
         <v>16</v>
@@ -17621,7 +17648,7 @@
     </row>
     <row r="840" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A840" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B840" s="1" t="s">
         <v>16</v>
@@ -17629,38 +17656,41 @@
       <c r="C840" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V840" s="1" t="s">
+      <c r="X840" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="841" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A841" s="1" t="s">
-        <v>947</v>
-      </c>
-      <c r="D841" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E841" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U841" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C841" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V841" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="842" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A842" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E842" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U842" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="843" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A843" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -17671,1405 +17701,1375 @@
     </row>
     <row r="844" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A844" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="D844" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E844" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="845" spans="1:1025" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A845" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="D844" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E844" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="845" spans="1:1025" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A845" s="9" t="s">
+      <c r="D845" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E845" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="846" spans="1:1025" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A846" s="9" t="s">
         <v>951</v>
       </c>
-      <c r="B845" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C845" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D845" s="9"/>
-      <c r="E845" s="9"/>
-      <c r="F845" s="9"/>
-      <c r="G845" s="9"/>
-      <c r="H845" s="9"/>
-      <c r="I845" s="9"/>
-      <c r="J845" s="9"/>
-      <c r="K845" s="9"/>
-      <c r="L845" s="9"/>
-      <c r="M845" s="9"/>
-      <c r="N845" s="9"/>
-      <c r="O845" s="9"/>
-      <c r="P845" s="9"/>
-      <c r="Q845" s="9"/>
-      <c r="R845" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="S845" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="T845" s="9"/>
-      <c r="U845" s="9"/>
-      <c r="V845" s="9"/>
-      <c r="W845" s="9"/>
-      <c r="X845" s="9"/>
-      <c r="Y845" s="9"/>
-      <c r="Z845" s="9"/>
-      <c r="AA845" s="9"/>
-      <c r="AB845" s="9"/>
-      <c r="AC845" s="9"/>
-      <c r="AD845" s="9"/>
-      <c r="AE845" s="9"/>
-      <c r="AF845" s="9"/>
-      <c r="AG845" s="9"/>
-      <c r="AH845" s="9"/>
-      <c r="AI845" s="9"/>
-      <c r="AJ845" s="9"/>
-      <c r="AK845" s="9"/>
-      <c r="AL845" s="9"/>
-      <c r="AM845" s="9"/>
-      <c r="AN845" s="9"/>
-      <c r="AO845" s="9"/>
-      <c r="AP845" s="9"/>
-      <c r="AQ845" s="9"/>
-      <c r="AR845" s="9"/>
-      <c r="AS845" s="9"/>
-      <c r="AT845" s="9"/>
-      <c r="AU845" s="9"/>
-      <c r="AV845" s="9"/>
-      <c r="AW845" s="9"/>
-      <c r="AX845" s="9"/>
-      <c r="AY845" s="9"/>
-      <c r="AZ845" s="9"/>
-      <c r="BA845" s="9"/>
-      <c r="BB845" s="9"/>
-      <c r="BC845" s="9"/>
-      <c r="BD845" s="9"/>
-      <c r="BE845" s="9"/>
-      <c r="BF845" s="9"/>
-      <c r="BG845" s="9"/>
-      <c r="BH845" s="9"/>
-      <c r="BI845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BJ845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BK845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BL845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BM845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BN845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BO845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BP845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BQ845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BR845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BS845" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="BT845" s="9"/>
-      <c r="BU845" s="9"/>
-      <c r="BV845" s="9"/>
-      <c r="BW845" s="9"/>
-      <c r="BX845" s="9"/>
-      <c r="BY845" s="9"/>
-      <c r="BZ845" s="9"/>
-      <c r="CA845" s="9"/>
-      <c r="CB845" s="9"/>
-      <c r="CC845" s="9"/>
-      <c r="CD845" s="9"/>
-      <c r="CE845" s="9"/>
-      <c r="CF845" s="9"/>
-      <c r="CG845" s="9"/>
-      <c r="CH845" s="9"/>
-      <c r="CI845" s="9"/>
-      <c r="CJ845" s="9"/>
-      <c r="CK845" s="9"/>
-      <c r="CL845" s="9"/>
-      <c r="CM845" s="9"/>
-      <c r="CN845" s="9"/>
-      <c r="CO845" s="9"/>
-      <c r="CP845" s="9"/>
-      <c r="CQ845" s="9"/>
-      <c r="CR845" s="9"/>
-      <c r="CS845" s="9"/>
-      <c r="CT845" s="9"/>
-      <c r="CU845" s="9"/>
-      <c r="CV845" s="9"/>
-      <c r="CW845" s="9"/>
-      <c r="CX845" s="9"/>
-      <c r="CY845" s="9"/>
-      <c r="CZ845" s="9"/>
-      <c r="DA845" s="9"/>
-      <c r="DB845" s="9"/>
-      <c r="DC845" s="9"/>
-      <c r="DD845" s="9"/>
-      <c r="DE845" s="9"/>
-      <c r="DF845" s="9"/>
-      <c r="DG845" s="9"/>
-      <c r="DH845" s="9"/>
-      <c r="DI845" s="9"/>
-      <c r="DJ845" s="9"/>
-      <c r="DK845" s="9"/>
-      <c r="DL845" s="9"/>
-      <c r="DM845" s="9"/>
-      <c r="DN845" s="9"/>
-      <c r="DO845" s="9"/>
-      <c r="DP845" s="9"/>
-      <c r="DQ845" s="9"/>
-      <c r="DR845" s="9"/>
-      <c r="DS845" s="9"/>
-      <c r="DT845" s="9"/>
-      <c r="DU845" s="9"/>
-      <c r="DV845" s="9"/>
-      <c r="DW845" s="9"/>
-      <c r="DX845" s="9"/>
-      <c r="DY845" s="9"/>
-      <c r="DZ845" s="9"/>
-      <c r="EA845" s="9"/>
-      <c r="EB845" s="9"/>
-      <c r="EC845" s="9"/>
-      <c r="ED845" s="9"/>
-      <c r="EE845" s="9"/>
-      <c r="EF845" s="9"/>
-      <c r="EG845" s="9"/>
-      <c r="EH845" s="9"/>
-      <c r="EI845" s="9"/>
-      <c r="EJ845" s="9"/>
-      <c r="EK845" s="9"/>
-      <c r="EL845" s="9"/>
-      <c r="EM845" s="9"/>
-      <c r="EN845" s="9"/>
-      <c r="EO845" s="9"/>
-      <c r="EP845" s="9"/>
-      <c r="EQ845" s="9"/>
-      <c r="ER845" s="9"/>
-      <c r="ES845" s="9"/>
-      <c r="ET845" s="9"/>
-      <c r="EU845" s="9"/>
-      <c r="EV845" s="9"/>
-      <c r="EW845" s="9"/>
-      <c r="EX845" s="9"/>
-      <c r="EY845" s="9"/>
-      <c r="EZ845" s="9"/>
-      <c r="FA845" s="9"/>
-      <c r="FB845" s="9"/>
-      <c r="FC845" s="9"/>
-      <c r="FD845" s="9"/>
-      <c r="FE845" s="9"/>
-      <c r="FF845" s="9"/>
-      <c r="FG845" s="9"/>
-      <c r="FH845" s="9"/>
-      <c r="FI845" s="9"/>
-      <c r="FJ845" s="9"/>
-      <c r="FK845" s="9"/>
-      <c r="FL845" s="9"/>
-      <c r="FM845" s="9"/>
-      <c r="FN845" s="9"/>
-      <c r="FO845" s="9"/>
-      <c r="FP845" s="9"/>
-      <c r="FQ845" s="9"/>
-      <c r="FR845" s="9"/>
-      <c r="FS845" s="9"/>
-      <c r="FT845" s="9"/>
-      <c r="FU845" s="9"/>
-      <c r="FV845" s="9"/>
-      <c r="FW845" s="9"/>
-      <c r="FX845" s="9"/>
-      <c r="FY845" s="9"/>
-      <c r="FZ845" s="9"/>
-      <c r="GA845" s="9"/>
-      <c r="GB845" s="9"/>
-      <c r="GC845" s="9"/>
-      <c r="GD845" s="9"/>
-      <c r="GE845" s="9"/>
-      <c r="GF845" s="9"/>
-      <c r="GG845" s="9"/>
-      <c r="GH845" s="9"/>
-      <c r="GI845" s="9"/>
-      <c r="GJ845" s="9"/>
-      <c r="GK845" s="9"/>
-      <c r="GL845" s="9"/>
-      <c r="GM845" s="9"/>
-      <c r="GN845" s="9"/>
-      <c r="GO845" s="9"/>
-      <c r="GP845" s="9"/>
-      <c r="GQ845" s="9"/>
-      <c r="GR845" s="9"/>
-      <c r="GS845" s="9"/>
-      <c r="GT845" s="9"/>
-      <c r="GU845" s="9"/>
-      <c r="GV845" s="9"/>
-      <c r="GW845" s="9"/>
-      <c r="GX845" s="9"/>
-      <c r="GY845" s="9"/>
-      <c r="GZ845" s="9"/>
-      <c r="HA845" s="9"/>
-      <c r="HB845" s="9"/>
-      <c r="HC845" s="9"/>
-      <c r="HD845" s="9"/>
-      <c r="HE845" s="9"/>
-      <c r="HF845" s="9"/>
-      <c r="HG845" s="9"/>
-      <c r="HH845" s="9"/>
-      <c r="HI845" s="9"/>
-      <c r="HJ845" s="9"/>
-      <c r="HK845" s="9"/>
-      <c r="HL845" s="9"/>
-      <c r="HM845" s="9"/>
-      <c r="HN845" s="9"/>
-      <c r="HO845" s="9"/>
-      <c r="HP845" s="9"/>
-      <c r="HQ845" s="9"/>
-      <c r="HR845" s="9"/>
-      <c r="HS845" s="9"/>
-      <c r="HT845" s="9"/>
-      <c r="HU845" s="9"/>
-      <c r="HV845" s="9"/>
-      <c r="HW845" s="9"/>
-      <c r="HX845" s="9"/>
-      <c r="HY845" s="9"/>
-      <c r="HZ845" s="9"/>
-      <c r="IA845" s="9"/>
-      <c r="IB845" s="9"/>
-      <c r="IC845" s="9"/>
-      <c r="ID845" s="9"/>
-      <c r="IE845" s="9"/>
-      <c r="IF845" s="9"/>
-      <c r="IG845" s="9"/>
-      <c r="IH845" s="9"/>
-      <c r="II845" s="9"/>
-      <c r="IJ845" s="9"/>
-      <c r="IK845" s="9"/>
-      <c r="IL845" s="9"/>
-      <c r="IM845" s="9"/>
-      <c r="IN845" s="9"/>
-      <c r="IO845" s="9"/>
-      <c r="IP845" s="9"/>
-      <c r="IQ845" s="9"/>
-      <c r="IR845" s="9"/>
-      <c r="IS845" s="9"/>
-      <c r="IT845" s="9"/>
-      <c r="IU845" s="9"/>
-      <c r="IV845" s="9"/>
-      <c r="IW845" s="9"/>
-      <c r="IX845" s="9"/>
-      <c r="IY845" s="9"/>
-      <c r="IZ845" s="9"/>
-      <c r="JA845" s="9"/>
-      <c r="JB845" s="9"/>
-      <c r="JC845" s="9"/>
-      <c r="JD845" s="9"/>
-      <c r="JE845" s="9"/>
-      <c r="JF845" s="9"/>
-      <c r="JG845" s="9"/>
-      <c r="JH845" s="9"/>
-      <c r="JI845" s="9"/>
-      <c r="JJ845" s="9"/>
-      <c r="JK845" s="9"/>
-      <c r="JL845" s="9"/>
-      <c r="JM845" s="9"/>
-      <c r="JN845" s="9"/>
-      <c r="JO845" s="9"/>
-      <c r="JP845" s="9"/>
-      <c r="JQ845" s="9"/>
-      <c r="JR845" s="9"/>
-      <c r="JS845" s="9"/>
-      <c r="JT845" s="9"/>
-      <c r="JU845" s="9"/>
-      <c r="JV845" s="9"/>
-      <c r="JW845" s="9"/>
-      <c r="JX845" s="9"/>
-      <c r="JY845" s="9"/>
-      <c r="JZ845" s="9"/>
-      <c r="KA845" s="9"/>
-      <c r="KB845" s="9"/>
-      <c r="KC845" s="9"/>
-      <c r="KD845" s="9"/>
-      <c r="KE845" s="9"/>
-      <c r="KF845" s="9"/>
-      <c r="KG845" s="9"/>
-      <c r="KH845" s="9"/>
-      <c r="KI845" s="9"/>
-      <c r="KJ845" s="9"/>
-      <c r="KK845" s="9"/>
-      <c r="KL845" s="9"/>
-      <c r="KM845" s="9"/>
-      <c r="KN845" s="9"/>
-      <c r="KO845" s="9"/>
-      <c r="KP845" s="9"/>
-      <c r="KQ845" s="9"/>
-      <c r="KR845" s="9"/>
-      <c r="KS845" s="9"/>
-      <c r="KT845" s="9"/>
-      <c r="KU845" s="9"/>
-      <c r="KV845" s="9"/>
-      <c r="KW845" s="9"/>
-      <c r="KX845" s="9"/>
-      <c r="KY845" s="9"/>
-      <c r="KZ845" s="9"/>
-      <c r="LA845" s="9"/>
-      <c r="LB845" s="9"/>
-      <c r="LC845" s="9"/>
-      <c r="LD845" s="9"/>
-      <c r="LE845" s="9"/>
-      <c r="LF845" s="9"/>
-      <c r="LG845" s="9"/>
-      <c r="LH845" s="9"/>
-      <c r="LI845" s="9"/>
-      <c r="LJ845" s="9"/>
-      <c r="LK845" s="9"/>
-      <c r="LL845" s="9"/>
-      <c r="LM845" s="9"/>
-      <c r="LN845" s="9"/>
-      <c r="LO845" s="9"/>
-      <c r="LP845" s="9"/>
-      <c r="LQ845" s="9"/>
-      <c r="LR845" s="9"/>
-      <c r="LS845" s="9"/>
-      <c r="LT845" s="9"/>
-      <c r="LU845" s="9"/>
-      <c r="LV845" s="9"/>
-      <c r="LW845" s="9"/>
-      <c r="LX845" s="9"/>
-      <c r="LY845" s="9"/>
-      <c r="LZ845" s="9"/>
-      <c r="MA845" s="9"/>
-      <c r="MB845" s="9"/>
-      <c r="MC845" s="9"/>
-      <c r="MD845" s="9"/>
-      <c r="ME845" s="9"/>
-      <c r="MF845" s="9"/>
-      <c r="MG845" s="9"/>
-      <c r="MH845" s="9"/>
-      <c r="MI845" s="9"/>
-      <c r="MJ845" s="9"/>
-      <c r="MK845" s="9"/>
-      <c r="ML845" s="9"/>
-      <c r="MM845" s="9"/>
-      <c r="MN845" s="9"/>
-      <c r="MO845" s="9"/>
-      <c r="MP845" s="9"/>
-      <c r="MQ845" s="9"/>
-      <c r="MR845" s="9"/>
-      <c r="MS845" s="9"/>
-      <c r="MT845" s="9"/>
-      <c r="MU845" s="9"/>
-      <c r="MV845" s="9"/>
-      <c r="MW845" s="9"/>
-      <c r="MX845" s="9"/>
-      <c r="MY845" s="9"/>
-      <c r="MZ845" s="9"/>
-      <c r="NA845" s="9"/>
-      <c r="NB845" s="9"/>
-      <c r="NC845" s="9"/>
-      <c r="ND845" s="9"/>
-      <c r="NE845" s="9"/>
-      <c r="NF845" s="9"/>
-      <c r="NG845" s="9"/>
-      <c r="NH845" s="9"/>
-      <c r="NI845" s="9"/>
-      <c r="NJ845" s="9"/>
-      <c r="NK845" s="9"/>
-      <c r="NL845" s="9"/>
-      <c r="NM845" s="9"/>
-      <c r="NN845" s="9"/>
-      <c r="NO845" s="9"/>
-      <c r="NP845" s="9"/>
-      <c r="NQ845" s="9"/>
-      <c r="NR845" s="9"/>
-      <c r="NS845" s="9"/>
-      <c r="NT845" s="9"/>
-      <c r="NU845" s="9"/>
-      <c r="NV845" s="9"/>
-      <c r="NW845" s="9"/>
-      <c r="NX845" s="9"/>
-      <c r="NY845" s="9"/>
-      <c r="NZ845" s="9"/>
-      <c r="OA845" s="9"/>
-      <c r="OB845" s="9"/>
-      <c r="OC845" s="9"/>
-      <c r="OD845" s="9"/>
-      <c r="OE845" s="9"/>
-      <c r="OF845" s="9"/>
-      <c r="OG845" s="9"/>
-      <c r="OH845" s="9"/>
-      <c r="OI845" s="9"/>
-      <c r="OJ845" s="9"/>
-      <c r="OK845" s="9"/>
-      <c r="OL845" s="9"/>
-      <c r="OM845" s="9"/>
-      <c r="ON845" s="9"/>
-      <c r="OO845" s="9"/>
-      <c r="OP845" s="9"/>
-      <c r="OQ845" s="9"/>
-      <c r="OR845" s="9"/>
-      <c r="OS845" s="9"/>
-      <c r="OT845" s="9"/>
-      <c r="OU845" s="9"/>
-      <c r="OV845" s="9"/>
-      <c r="OW845" s="9"/>
-      <c r="OX845" s="9"/>
-      <c r="OY845" s="9"/>
-      <c r="OZ845" s="9"/>
-      <c r="PA845" s="9"/>
-      <c r="PB845" s="9"/>
-      <c r="PC845" s="9"/>
-      <c r="PD845" s="9"/>
-      <c r="PE845" s="9"/>
-      <c r="PF845" s="9"/>
-      <c r="PG845" s="9"/>
-      <c r="PH845" s="9"/>
-      <c r="PI845" s="9"/>
-      <c r="PJ845" s="9"/>
-      <c r="PK845" s="9"/>
-      <c r="PL845" s="9"/>
-      <c r="PM845" s="9"/>
-      <c r="PN845" s="9"/>
-      <c r="PO845" s="9"/>
-      <c r="PP845" s="9"/>
-      <c r="PQ845" s="9"/>
-      <c r="PR845" s="9"/>
-      <c r="PS845" s="9"/>
-      <c r="PT845" s="9"/>
-      <c r="PU845" s="9"/>
-      <c r="PV845" s="9"/>
-      <c r="PW845" s="9"/>
-      <c r="PX845" s="9"/>
-      <c r="PY845" s="9"/>
-      <c r="PZ845" s="9"/>
-      <c r="QA845" s="9"/>
-      <c r="QB845" s="9"/>
-      <c r="QC845" s="9"/>
-      <c r="QD845" s="9"/>
-      <c r="QE845" s="9"/>
-      <c r="QF845" s="9"/>
-      <c r="QG845" s="9"/>
-      <c r="QH845" s="9"/>
-      <c r="QI845" s="9"/>
-      <c r="QJ845" s="9"/>
-      <c r="QK845" s="9"/>
-      <c r="QL845" s="9"/>
-      <c r="QM845" s="9"/>
-      <c r="QN845" s="9"/>
-      <c r="QO845" s="9"/>
-      <c r="QP845" s="9"/>
-      <c r="QQ845" s="9"/>
-      <c r="QR845" s="9"/>
-      <c r="QS845" s="9"/>
-      <c r="QT845" s="9"/>
-      <c r="QU845" s="9"/>
-      <c r="QV845" s="9"/>
-      <c r="QW845" s="9"/>
-      <c r="QX845" s="9"/>
-      <c r="QY845" s="9"/>
-      <c r="QZ845" s="9"/>
-      <c r="RA845" s="9"/>
-      <c r="RB845" s="9"/>
-      <c r="RC845" s="9"/>
-      <c r="RD845" s="9"/>
-      <c r="RE845" s="9"/>
-      <c r="RF845" s="9"/>
-      <c r="RG845" s="9"/>
-      <c r="RH845" s="9"/>
-      <c r="RI845" s="9"/>
-      <c r="RJ845" s="9"/>
-      <c r="RK845" s="9"/>
-      <c r="RL845" s="9"/>
-      <c r="RM845" s="9"/>
-      <c r="RN845" s="9"/>
-      <c r="RO845" s="9"/>
-      <c r="RP845" s="9"/>
-      <c r="RQ845" s="9"/>
-      <c r="RR845" s="9"/>
-      <c r="RS845" s="9"/>
-      <c r="RT845" s="9"/>
-      <c r="RU845" s="9"/>
-      <c r="RV845" s="9"/>
-      <c r="RW845" s="9"/>
-      <c r="RX845" s="9"/>
-      <c r="RY845" s="9"/>
-      <c r="RZ845" s="9"/>
-      <c r="SA845" s="9"/>
-      <c r="SB845" s="9"/>
-      <c r="SC845" s="9"/>
-      <c r="SD845" s="9"/>
-      <c r="SE845" s="9"/>
-      <c r="SF845" s="9"/>
-      <c r="SG845" s="9"/>
-      <c r="SH845" s="9"/>
-      <c r="SI845" s="9"/>
-      <c r="SJ845" s="9"/>
-      <c r="SK845" s="9"/>
-      <c r="SL845" s="9"/>
-      <c r="SM845" s="9"/>
-      <c r="SN845" s="9"/>
-      <c r="SO845" s="9"/>
-      <c r="SP845" s="9"/>
-      <c r="SQ845" s="9"/>
-      <c r="SR845" s="9"/>
-      <c r="SS845" s="9"/>
-      <c r="ST845" s="9"/>
-      <c r="SU845" s="9"/>
-      <c r="SV845" s="9"/>
-      <c r="SW845" s="9"/>
-      <c r="SX845" s="9"/>
-      <c r="SY845" s="9"/>
-      <c r="SZ845" s="9"/>
-      <c r="TA845" s="9"/>
-      <c r="TB845" s="9"/>
-      <c r="TC845" s="9"/>
-      <c r="TD845" s="9"/>
-      <c r="TE845" s="9"/>
-      <c r="TF845" s="9"/>
-      <c r="TG845" s="9"/>
-      <c r="TH845" s="9"/>
-      <c r="TI845" s="9"/>
-      <c r="TJ845" s="9"/>
-      <c r="TK845" s="9"/>
-      <c r="TL845" s="9"/>
-      <c r="TM845" s="9"/>
-      <c r="TN845" s="9"/>
-      <c r="TO845" s="9"/>
-      <c r="TP845" s="9"/>
-      <c r="TQ845" s="9"/>
-      <c r="TR845" s="9"/>
-      <c r="TS845" s="9"/>
-      <c r="TT845" s="9"/>
-      <c r="TU845" s="9"/>
-      <c r="TV845" s="9"/>
-      <c r="TW845" s="9"/>
-      <c r="TX845" s="9"/>
-      <c r="TY845" s="9"/>
-      <c r="TZ845" s="9"/>
-      <c r="UA845" s="9"/>
-      <c r="UB845" s="9"/>
-      <c r="UC845" s="9"/>
-      <c r="UD845" s="9"/>
-      <c r="UE845" s="9"/>
-      <c r="UF845" s="9"/>
-      <c r="UG845" s="9"/>
-      <c r="UH845" s="9"/>
-      <c r="UI845" s="9"/>
-      <c r="UJ845" s="9"/>
-      <c r="UK845" s="9"/>
-      <c r="UL845" s="9"/>
-      <c r="UM845" s="9"/>
-      <c r="UN845" s="9"/>
-      <c r="UO845" s="9"/>
-      <c r="UP845" s="9"/>
-      <c r="UQ845" s="9"/>
-      <c r="UR845" s="9"/>
-      <c r="US845" s="9"/>
-      <c r="UT845" s="9"/>
-      <c r="UU845" s="9"/>
-      <c r="UV845" s="9"/>
-      <c r="UW845" s="9"/>
-      <c r="UX845" s="9"/>
-      <c r="UY845" s="9"/>
-      <c r="UZ845" s="9"/>
-      <c r="VA845" s="9"/>
-      <c r="VB845" s="9"/>
-      <c r="VC845" s="9"/>
-      <c r="VD845" s="9"/>
-      <c r="VE845" s="9"/>
-      <c r="VF845" s="9"/>
-      <c r="VG845" s="9"/>
-      <c r="VH845" s="9"/>
-      <c r="VI845" s="9"/>
-      <c r="VJ845" s="9"/>
-      <c r="VK845" s="9"/>
-      <c r="VL845" s="9"/>
-      <c r="VM845" s="9"/>
-      <c r="VN845" s="9"/>
-      <c r="VO845" s="9"/>
-      <c r="VP845" s="9"/>
-      <c r="VQ845" s="9"/>
-      <c r="VR845" s="9"/>
-      <c r="VS845" s="9"/>
-      <c r="VT845" s="9"/>
-      <c r="VU845" s="9"/>
-      <c r="VV845" s="9"/>
-      <c r="VW845" s="9"/>
-      <c r="VX845" s="9"/>
-      <c r="VY845" s="9"/>
-      <c r="VZ845" s="9"/>
-      <c r="WA845" s="9"/>
-      <c r="WB845" s="9"/>
-      <c r="WC845" s="9"/>
-      <c r="WD845" s="9"/>
-      <c r="WE845" s="9"/>
-      <c r="WF845" s="9"/>
-      <c r="WG845" s="9"/>
-      <c r="WH845" s="9"/>
-      <c r="WI845" s="9"/>
-      <c r="WJ845" s="9"/>
-      <c r="WK845" s="9"/>
-      <c r="WL845" s="9"/>
-      <c r="WM845" s="9"/>
-      <c r="WN845" s="9"/>
-      <c r="WO845" s="9"/>
-      <c r="WP845" s="9"/>
-      <c r="WQ845" s="9"/>
-      <c r="WR845" s="9"/>
-      <c r="WS845" s="9"/>
-      <c r="WT845" s="9"/>
-      <c r="WU845" s="9"/>
-      <c r="WV845" s="9"/>
-      <c r="WW845" s="9"/>
-      <c r="WX845" s="9"/>
-      <c r="WY845" s="9"/>
-      <c r="WZ845" s="9"/>
-      <c r="XA845" s="9"/>
-      <c r="XB845" s="9"/>
-      <c r="XC845" s="9"/>
-      <c r="XD845" s="9"/>
-      <c r="XE845" s="9"/>
-      <c r="XF845" s="9"/>
-      <c r="XG845" s="9"/>
-      <c r="XH845" s="9"/>
-      <c r="XI845" s="9"/>
-      <c r="XJ845" s="9"/>
-      <c r="XK845" s="9"/>
-      <c r="XL845" s="9"/>
-      <c r="XM845" s="9"/>
-      <c r="XN845" s="9"/>
-      <c r="XO845" s="9"/>
-      <c r="XP845" s="9"/>
-      <c r="XQ845" s="9"/>
-      <c r="XR845" s="9"/>
-      <c r="XS845" s="9"/>
-      <c r="XT845" s="9"/>
-      <c r="XU845" s="9"/>
-      <c r="XV845" s="9"/>
-      <c r="XW845" s="9"/>
-      <c r="XX845" s="9"/>
-      <c r="XY845" s="9"/>
-      <c r="XZ845" s="9"/>
-      <c r="YA845" s="9"/>
-      <c r="YB845" s="9"/>
-      <c r="YC845" s="9"/>
-      <c r="YD845" s="9"/>
-      <c r="YE845" s="9"/>
-      <c r="YF845" s="9"/>
-      <c r="YG845" s="9"/>
-      <c r="YH845" s="9"/>
-      <c r="YI845" s="9"/>
-      <c r="YJ845" s="9"/>
-      <c r="YK845" s="9"/>
-      <c r="YL845" s="9"/>
-      <c r="YM845" s="9"/>
-      <c r="YN845" s="9"/>
-      <c r="YO845" s="9"/>
-      <c r="YP845" s="9"/>
-      <c r="YQ845" s="9"/>
-      <c r="YR845" s="9"/>
-      <c r="YS845" s="9"/>
-      <c r="YT845" s="9"/>
-      <c r="YU845" s="9"/>
-      <c r="YV845" s="9"/>
-      <c r="YW845" s="9"/>
-      <c r="YX845" s="9"/>
-      <c r="YY845" s="9"/>
-      <c r="YZ845" s="9"/>
-      <c r="ZA845" s="9"/>
-      <c r="ZB845" s="9"/>
-      <c r="ZC845" s="9"/>
-      <c r="ZD845" s="9"/>
-      <c r="ZE845" s="9"/>
-      <c r="ZF845" s="9"/>
-      <c r="ZG845" s="9"/>
-      <c r="ZH845" s="9"/>
-      <c r="ZI845" s="9"/>
-      <c r="ZJ845" s="9"/>
-      <c r="ZK845" s="9"/>
-      <c r="ZL845" s="9"/>
-      <c r="ZM845" s="9"/>
-      <c r="ZN845" s="9"/>
-      <c r="ZO845" s="9"/>
-      <c r="ZP845" s="9"/>
-      <c r="ZQ845" s="9"/>
-      <c r="ZR845" s="9"/>
-      <c r="ZS845" s="9"/>
-      <c r="ZT845" s="9"/>
-      <c r="ZU845" s="9"/>
-      <c r="ZV845" s="9"/>
-      <c r="ZW845" s="9"/>
-      <c r="ZX845" s="9"/>
-      <c r="ZY845" s="9"/>
-      <c r="ZZ845" s="9"/>
-      <c r="AAA845" s="9"/>
-      <c r="AAB845" s="9"/>
-      <c r="AAC845" s="9"/>
-      <c r="AAD845" s="9"/>
-      <c r="AAE845" s="9"/>
-      <c r="AAF845" s="9"/>
-      <c r="AAG845" s="9"/>
-      <c r="AAH845" s="9"/>
-      <c r="AAI845" s="9"/>
-      <c r="AAJ845" s="9"/>
-      <c r="AAK845" s="9"/>
-      <c r="AAL845" s="9"/>
-      <c r="AAM845" s="9"/>
-      <c r="AAN845" s="9"/>
-      <c r="AAO845" s="9"/>
-      <c r="AAP845" s="9"/>
-      <c r="AAQ845" s="9"/>
-      <c r="AAR845" s="9"/>
-      <c r="AAS845" s="9"/>
-      <c r="AAT845" s="9"/>
-      <c r="AAU845" s="9"/>
-      <c r="AAV845" s="9"/>
-      <c r="AAW845" s="9"/>
-      <c r="AAX845" s="9"/>
-      <c r="AAY845" s="9"/>
-      <c r="AAZ845" s="9"/>
-      <c r="ABA845" s="9"/>
-      <c r="ABB845" s="9"/>
-      <c r="ABC845" s="9"/>
-      <c r="ABD845" s="9"/>
-      <c r="ABE845" s="9"/>
-      <c r="ABF845" s="9"/>
-      <c r="ABG845" s="9"/>
-      <c r="ABH845" s="9"/>
-      <c r="ABI845" s="9"/>
-      <c r="ABJ845" s="9"/>
-      <c r="ABK845" s="9"/>
-      <c r="ABL845" s="9"/>
-      <c r="ABM845" s="9"/>
-      <c r="ABN845" s="9"/>
-      <c r="ABO845" s="9"/>
-      <c r="ABP845" s="9"/>
-      <c r="ABQ845" s="9"/>
-      <c r="ABR845" s="9"/>
-      <c r="ABS845" s="9"/>
-      <c r="ABT845" s="9"/>
-      <c r="ABU845" s="9"/>
-      <c r="ABV845" s="9"/>
-      <c r="ABW845" s="9"/>
-      <c r="ABX845" s="9"/>
-      <c r="ABY845" s="9"/>
-      <c r="ABZ845" s="9"/>
-      <c r="ACA845" s="9"/>
-      <c r="ACB845" s="9"/>
-      <c r="ACC845" s="9"/>
-      <c r="ACD845" s="9"/>
-      <c r="ACE845" s="9"/>
-      <c r="ACF845" s="9"/>
-      <c r="ACG845" s="9"/>
-      <c r="ACH845" s="9"/>
-      <c r="ACI845" s="9"/>
-      <c r="ACJ845" s="9"/>
-      <c r="ACK845" s="9"/>
-      <c r="ACL845" s="9"/>
-      <c r="ACM845" s="9"/>
-      <c r="ACN845" s="9"/>
-      <c r="ACO845" s="9"/>
-      <c r="ACP845" s="9"/>
-      <c r="ACQ845" s="9"/>
-      <c r="ACR845" s="9"/>
-      <c r="ACS845" s="9"/>
-      <c r="ACT845" s="9"/>
-      <c r="ACU845" s="9"/>
-      <c r="ACV845" s="9"/>
-      <c r="ACW845" s="9"/>
-      <c r="ACX845" s="9"/>
-      <c r="ACY845" s="9"/>
-      <c r="ACZ845" s="9"/>
-      <c r="ADA845" s="9"/>
-      <c r="ADB845" s="9"/>
-      <c r="ADC845" s="9"/>
-      <c r="ADD845" s="9"/>
-      <c r="ADE845" s="9"/>
-      <c r="ADF845" s="9"/>
-      <c r="ADG845" s="9"/>
-      <c r="ADH845" s="9"/>
-      <c r="ADI845" s="9"/>
-      <c r="ADJ845" s="9"/>
-      <c r="ADK845" s="9"/>
-      <c r="ADL845" s="9"/>
-      <c r="ADM845" s="9"/>
-      <c r="ADN845" s="9"/>
-      <c r="ADO845" s="9"/>
-      <c r="ADP845" s="9"/>
-      <c r="ADQ845" s="9"/>
-      <c r="ADR845" s="9"/>
-      <c r="ADS845" s="9"/>
-      <c r="ADT845" s="9"/>
-      <c r="ADU845" s="9"/>
-      <c r="ADV845" s="9"/>
-      <c r="ADW845" s="9"/>
-      <c r="ADX845" s="9"/>
-      <c r="ADY845" s="9"/>
-      <c r="ADZ845" s="9"/>
-      <c r="AEA845" s="9"/>
-      <c r="AEB845" s="9"/>
-      <c r="AEC845" s="9"/>
-      <c r="AED845" s="9"/>
-      <c r="AEE845" s="9"/>
-      <c r="AEF845" s="9"/>
-      <c r="AEG845" s="9"/>
-      <c r="AEH845" s="9"/>
-      <c r="AEI845" s="9"/>
-      <c r="AEJ845" s="9"/>
-      <c r="AEK845" s="9"/>
-      <c r="AEL845" s="9"/>
-      <c r="AEM845" s="9"/>
-      <c r="AEN845" s="9"/>
-      <c r="AEO845" s="9"/>
-      <c r="AEP845" s="9"/>
-      <c r="AEQ845" s="9"/>
-      <c r="AER845" s="9"/>
-      <c r="AES845" s="9"/>
-      <c r="AET845" s="9"/>
-      <c r="AEU845" s="9"/>
-      <c r="AEV845" s="9"/>
-      <c r="AEW845" s="9"/>
-      <c r="AEX845" s="9"/>
-      <c r="AEY845" s="9"/>
-      <c r="AEZ845" s="9"/>
-      <c r="AFA845" s="9"/>
-      <c r="AFB845" s="9"/>
-      <c r="AFC845" s="9"/>
-      <c r="AFD845" s="9"/>
-      <c r="AFE845" s="9"/>
-      <c r="AFF845" s="9"/>
-      <c r="AFG845" s="9"/>
-      <c r="AFH845" s="9"/>
-      <c r="AFI845" s="9"/>
-      <c r="AFJ845" s="9"/>
-      <c r="AFK845" s="9"/>
-      <c r="AFL845" s="9"/>
-      <c r="AFM845" s="9"/>
-      <c r="AFN845" s="9"/>
-      <c r="AFO845" s="9"/>
-      <c r="AFP845" s="9"/>
-      <c r="AFQ845" s="9"/>
-      <c r="AFR845" s="9"/>
-      <c r="AFS845" s="9"/>
-      <c r="AFT845" s="9"/>
-      <c r="AFU845" s="9"/>
-      <c r="AFV845" s="9"/>
-      <c r="AFW845" s="9"/>
-      <c r="AFX845" s="9"/>
-      <c r="AFY845" s="9"/>
-      <c r="AFZ845" s="9"/>
-      <c r="AGA845" s="9"/>
-      <c r="AGB845" s="9"/>
-      <c r="AGC845" s="9"/>
-      <c r="AGD845" s="9"/>
-      <c r="AGE845" s="9"/>
-      <c r="AGF845" s="9"/>
-      <c r="AGG845" s="9"/>
-      <c r="AGH845" s="9"/>
-      <c r="AGI845" s="9"/>
-      <c r="AGJ845" s="9"/>
-      <c r="AGK845" s="9"/>
-      <c r="AGL845" s="9"/>
-      <c r="AGM845" s="9"/>
-      <c r="AGN845" s="9"/>
-      <c r="AGO845" s="9"/>
-      <c r="AGP845" s="9"/>
-      <c r="AGQ845" s="9"/>
-      <c r="AGR845" s="9"/>
-      <c r="AGS845" s="9"/>
-      <c r="AGT845" s="9"/>
-      <c r="AGU845" s="9"/>
-      <c r="AGV845" s="9"/>
-      <c r="AGW845" s="9"/>
-      <c r="AGX845" s="9"/>
-      <c r="AGY845" s="9"/>
-      <c r="AGZ845" s="9"/>
-      <c r="AHA845" s="9"/>
-      <c r="AHB845" s="9"/>
-      <c r="AHC845" s="9"/>
-      <c r="AHD845" s="9"/>
-      <c r="AHE845" s="9"/>
-      <c r="AHF845" s="9"/>
-      <c r="AHG845" s="9"/>
-      <c r="AHH845" s="9"/>
-      <c r="AHI845" s="9"/>
-      <c r="AHJ845" s="9"/>
-      <c r="AHK845" s="9"/>
-      <c r="AHL845" s="9"/>
-      <c r="AHM845" s="9"/>
-      <c r="AHN845" s="9"/>
-      <c r="AHO845" s="9"/>
-      <c r="AHP845" s="9"/>
-      <c r="AHQ845" s="9"/>
-      <c r="AHR845" s="9"/>
-      <c r="AHS845" s="9"/>
-      <c r="AHT845" s="9"/>
-      <c r="AHU845" s="9"/>
-      <c r="AHV845" s="9"/>
-      <c r="AHW845" s="9"/>
-      <c r="AHX845" s="9"/>
-      <c r="AHY845" s="9"/>
-      <c r="AHZ845" s="9"/>
-      <c r="AIA845" s="9"/>
-      <c r="AIB845" s="9"/>
-      <c r="AIC845" s="9"/>
-      <c r="AID845" s="9"/>
-      <c r="AIE845" s="9"/>
-      <c r="AIF845" s="9"/>
-      <c r="AIG845" s="9"/>
-      <c r="AIH845" s="9"/>
-      <c r="AII845" s="9"/>
-      <c r="AIJ845" s="9"/>
-      <c r="AIK845" s="9"/>
-      <c r="AIL845" s="9"/>
-      <c r="AIM845" s="9"/>
-      <c r="AIN845" s="9"/>
-      <c r="AIO845" s="9"/>
-      <c r="AIP845" s="9"/>
-      <c r="AIQ845" s="9"/>
-      <c r="AIR845" s="9"/>
-      <c r="AIS845" s="9"/>
-      <c r="AIT845" s="9"/>
-      <c r="AIU845" s="9"/>
-      <c r="AIV845" s="9"/>
-      <c r="AIW845" s="9"/>
-      <c r="AIX845" s="9"/>
-      <c r="AIY845" s="9"/>
-      <c r="AIZ845" s="9"/>
-      <c r="AJA845" s="9"/>
-      <c r="AJB845" s="9"/>
-      <c r="AJC845" s="9"/>
-      <c r="AJD845" s="9"/>
-      <c r="AJE845" s="9"/>
-      <c r="AJF845" s="9"/>
-      <c r="AJG845" s="9"/>
-      <c r="AJH845" s="9"/>
-      <c r="AJI845" s="9"/>
-      <c r="AJJ845" s="9"/>
-      <c r="AJK845" s="9"/>
-      <c r="AJL845" s="9"/>
-      <c r="AJM845" s="9"/>
-      <c r="AJN845" s="9"/>
-      <c r="AJO845" s="9"/>
-      <c r="AJP845" s="9"/>
-      <c r="AJQ845" s="9"/>
-      <c r="AJR845" s="9"/>
-      <c r="AJS845" s="9"/>
-      <c r="AJT845" s="9"/>
-      <c r="AJU845" s="9"/>
-      <c r="AJV845" s="9"/>
-      <c r="AJW845" s="9"/>
-      <c r="AJX845" s="9"/>
-      <c r="AJY845" s="9"/>
-      <c r="AJZ845" s="9"/>
-      <c r="AKA845" s="9"/>
-      <c r="AKB845" s="9"/>
-      <c r="AKC845" s="9"/>
-      <c r="AKD845" s="9"/>
-      <c r="AKE845" s="9"/>
-      <c r="AKF845" s="9"/>
-      <c r="AKG845" s="9"/>
-      <c r="AKH845" s="9"/>
-      <c r="AKI845" s="9"/>
-      <c r="AKJ845" s="9"/>
-      <c r="AKK845" s="9"/>
-      <c r="AKL845" s="9"/>
-      <c r="AKM845" s="9"/>
-      <c r="AKN845" s="9"/>
-      <c r="AKO845" s="9"/>
-      <c r="AKP845" s="9"/>
-      <c r="AKQ845" s="9"/>
-      <c r="AKR845" s="9"/>
-      <c r="AKS845" s="9"/>
-      <c r="AKT845" s="9"/>
-      <c r="AKU845" s="9"/>
-      <c r="AKV845" s="9"/>
-      <c r="AKW845" s="9"/>
-      <c r="AKX845" s="9"/>
-      <c r="AKY845" s="9"/>
-      <c r="AKZ845" s="9"/>
-      <c r="ALA845" s="9"/>
-      <c r="ALB845" s="9"/>
-      <c r="ALC845" s="9"/>
-      <c r="ALD845" s="9"/>
-      <c r="ALE845" s="9"/>
-      <c r="ALF845" s="9"/>
-      <c r="ALG845" s="9"/>
-      <c r="ALH845" s="9"/>
-      <c r="ALI845" s="9"/>
-      <c r="ALJ845" s="9"/>
-      <c r="ALK845" s="9"/>
-      <c r="ALL845" s="9"/>
-      <c r="ALM845" s="9"/>
-      <c r="ALN845" s="9"/>
-      <c r="ALO845" s="9"/>
-      <c r="ALP845" s="9"/>
-      <c r="ALQ845" s="9"/>
-      <c r="ALR845" s="9"/>
-      <c r="ALS845" s="9"/>
-      <c r="ALT845" s="9"/>
-      <c r="ALU845" s="9"/>
-      <c r="ALV845" s="9"/>
-      <c r="ALW845" s="9"/>
-      <c r="ALX845" s="9"/>
-      <c r="ALY845" s="9"/>
-      <c r="ALZ845" s="9"/>
-      <c r="AMA845" s="9"/>
-      <c r="AMB845" s="9"/>
-      <c r="AMC845" s="9"/>
-      <c r="AMD845" s="9"/>
-      <c r="AME845" s="9"/>
-      <c r="AMF845" s="9"/>
-      <c r="AMG845" s="9"/>
-      <c r="AMH845" s="9"/>
-      <c r="AMI845" s="9"/>
-      <c r="AMJ845" s="9"/>
-      <c r="AMK845" s="9"/>
-    </row>
-    <row r="846" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A846" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="AI846" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ846" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B846" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C846" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D846" s="9"/>
+      <c r="E846" s="9"/>
+      <c r="F846" s="9"/>
+      <c r="G846" s="9"/>
+      <c r="H846" s="9"/>
+      <c r="I846" s="9"/>
+      <c r="J846" s="9"/>
+      <c r="K846" s="9"/>
+      <c r="L846" s="9"/>
+      <c r="M846" s="9"/>
+      <c r="N846" s="9"/>
+      <c r="O846" s="9"/>
+      <c r="P846" s="9"/>
+      <c r="Q846" s="9"/>
+      <c r="R846" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S846" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T846" s="9"/>
+      <c r="U846" s="9"/>
+      <c r="V846" s="9"/>
+      <c r="W846" s="9"/>
+      <c r="X846" s="9"/>
+      <c r="Y846" s="9"/>
+      <c r="Z846" s="9"/>
+      <c r="AA846" s="9"/>
+      <c r="AB846" s="9"/>
+      <c r="AC846" s="9"/>
+      <c r="AD846" s="9"/>
+      <c r="AE846" s="9"/>
+      <c r="AF846" s="9"/>
+      <c r="AG846" s="9"/>
+      <c r="AH846" s="9"/>
+      <c r="AI846" s="9"/>
+      <c r="AJ846" s="9"/>
+      <c r="AK846" s="9"/>
+      <c r="AL846" s="9"/>
+      <c r="AM846" s="9"/>
+      <c r="AN846" s="9"/>
+      <c r="AO846" s="9"/>
+      <c r="AP846" s="9"/>
+      <c r="AQ846" s="9"/>
+      <c r="AR846" s="9"/>
+      <c r="AS846" s="9"/>
+      <c r="AT846" s="9"/>
+      <c r="AU846" s="9"/>
+      <c r="AV846" s="9"/>
+      <c r="AW846" s="9"/>
+      <c r="AX846" s="9"/>
+      <c r="AY846" s="9"/>
+      <c r="AZ846" s="9"/>
+      <c r="BA846" s="9"/>
+      <c r="BB846" s="9"/>
+      <c r="BC846" s="9"/>
+      <c r="BD846" s="9"/>
+      <c r="BE846" s="9"/>
+      <c r="BF846" s="9"/>
+      <c r="BG846" s="9"/>
+      <c r="BH846" s="9"/>
+      <c r="BT846" s="9"/>
+      <c r="BU846" s="9"/>
+      <c r="BV846" s="9"/>
+      <c r="BW846" s="9"/>
+      <c r="BX846" s="9"/>
+      <c r="BY846" s="9"/>
+      <c r="BZ846" s="9"/>
+      <c r="CA846" s="9"/>
+      <c r="CB846" s="9"/>
+      <c r="CC846" s="9"/>
+      <c r="CD846" s="9"/>
+      <c r="CE846" s="9"/>
+      <c r="CF846" s="9"/>
+      <c r="CG846" s="9"/>
+      <c r="CH846" s="9"/>
+      <c r="CI846" s="9"/>
+      <c r="CJ846" s="9"/>
+      <c r="CK846" s="9"/>
+      <c r="CL846" s="9"/>
+      <c r="CM846" s="9"/>
+      <c r="CN846" s="9"/>
+      <c r="CO846" s="9"/>
+      <c r="CP846" s="9"/>
+      <c r="CQ846" s="9"/>
+      <c r="CR846" s="9"/>
+      <c r="CS846" s="9"/>
+      <c r="CT846" s="9"/>
+      <c r="CU846" s="9"/>
+      <c r="CV846" s="9"/>
+      <c r="CW846" s="9"/>
+      <c r="CX846" s="9"/>
+      <c r="CY846" s="9"/>
+      <c r="CZ846" s="9"/>
+      <c r="DA846" s="9"/>
+      <c r="DB846" s="9"/>
+      <c r="DC846" s="9"/>
+      <c r="DD846" s="9"/>
+      <c r="DE846" s="9"/>
+      <c r="DF846" s="9"/>
+      <c r="DG846" s="9"/>
+      <c r="DH846" s="9"/>
+      <c r="DI846" s="9"/>
+      <c r="DJ846" s="9"/>
+      <c r="DK846" s="9"/>
+      <c r="DL846" s="9"/>
+      <c r="DM846" s="9"/>
+      <c r="DN846" s="9"/>
+      <c r="DO846" s="9"/>
+      <c r="DP846" s="9"/>
+      <c r="DQ846" s="9"/>
+      <c r="DR846" s="9"/>
+      <c r="DS846" s="9"/>
+      <c r="DT846" s="9"/>
+      <c r="DU846" s="9"/>
+      <c r="DV846" s="9"/>
+      <c r="DW846" s="9"/>
+      <c r="DX846" s="9"/>
+      <c r="DY846" s="9"/>
+      <c r="DZ846" s="9"/>
+      <c r="EA846" s="9"/>
+      <c r="EB846" s="9"/>
+      <c r="EC846" s="9"/>
+      <c r="ED846" s="9"/>
+      <c r="EE846" s="9"/>
+      <c r="EF846" s="9"/>
+      <c r="EG846" s="9"/>
+      <c r="EH846" s="9"/>
+      <c r="EI846" s="9"/>
+      <c r="EJ846" s="9"/>
+      <c r="EK846" s="9"/>
+      <c r="EL846" s="9"/>
+      <c r="EM846" s="9"/>
+      <c r="EN846" s="9"/>
+      <c r="EO846" s="9"/>
+      <c r="EP846" s="9"/>
+      <c r="EQ846" s="9"/>
+      <c r="ER846" s="9"/>
+      <c r="ES846" s="9"/>
+      <c r="ET846" s="9"/>
+      <c r="EU846" s="9"/>
+      <c r="EV846" s="9"/>
+      <c r="EW846" s="9"/>
+      <c r="EX846" s="9"/>
+      <c r="EY846" s="9"/>
+      <c r="EZ846" s="9"/>
+      <c r="FA846" s="9"/>
+      <c r="FB846" s="9"/>
+      <c r="FC846" s="9"/>
+      <c r="FD846" s="9"/>
+      <c r="FE846" s="9"/>
+      <c r="FF846" s="9"/>
+      <c r="FG846" s="9"/>
+      <c r="FH846" s="9"/>
+      <c r="FI846" s="9"/>
+      <c r="FJ846" s="9"/>
+      <c r="FK846" s="9"/>
+      <c r="FL846" s="9"/>
+      <c r="FM846" s="9"/>
+      <c r="FN846" s="9"/>
+      <c r="FO846" s="9"/>
+      <c r="FP846" s="9"/>
+      <c r="FQ846" s="9"/>
+      <c r="FR846" s="9"/>
+      <c r="FS846" s="9"/>
+      <c r="FT846" s="9"/>
+      <c r="FU846" s="9"/>
+      <c r="FV846" s="9"/>
+      <c r="FW846" s="9"/>
+      <c r="FX846" s="9"/>
+      <c r="FY846" s="9"/>
+      <c r="FZ846" s="9"/>
+      <c r="GA846" s="9"/>
+      <c r="GB846" s="9"/>
+      <c r="GC846" s="9"/>
+      <c r="GD846" s="9"/>
+      <c r="GE846" s="9"/>
+      <c r="GF846" s="9"/>
+      <c r="GG846" s="9"/>
+      <c r="GH846" s="9"/>
+      <c r="GI846" s="9"/>
+      <c r="GJ846" s="9"/>
+      <c r="GK846" s="9"/>
+      <c r="GL846" s="9"/>
+      <c r="GM846" s="9"/>
+      <c r="GN846" s="9"/>
+      <c r="GO846" s="9"/>
+      <c r="GP846" s="9"/>
+      <c r="GQ846" s="9"/>
+      <c r="GR846" s="9"/>
+      <c r="GS846" s="9"/>
+      <c r="GT846" s="9"/>
+      <c r="GU846" s="9"/>
+      <c r="GV846" s="9"/>
+      <c r="GW846" s="9"/>
+      <c r="GX846" s="9"/>
+      <c r="GY846" s="9"/>
+      <c r="GZ846" s="9"/>
+      <c r="HA846" s="9"/>
+      <c r="HB846" s="9"/>
+      <c r="HC846" s="9"/>
+      <c r="HD846" s="9"/>
+      <c r="HE846" s="9"/>
+      <c r="HF846" s="9"/>
+      <c r="HG846" s="9"/>
+      <c r="HH846" s="9"/>
+      <c r="HI846" s="9"/>
+      <c r="HJ846" s="9"/>
+      <c r="HK846" s="9"/>
+      <c r="HL846" s="9"/>
+      <c r="HM846" s="9"/>
+      <c r="HN846" s="9"/>
+      <c r="HO846" s="9"/>
+      <c r="HP846" s="9"/>
+      <c r="HQ846" s="9"/>
+      <c r="HR846" s="9"/>
+      <c r="HS846" s="9"/>
+      <c r="HT846" s="9"/>
+      <c r="HU846" s="9"/>
+      <c r="HV846" s="9"/>
+      <c r="HW846" s="9"/>
+      <c r="HX846" s="9"/>
+      <c r="HY846" s="9"/>
+      <c r="HZ846" s="9"/>
+      <c r="IA846" s="9"/>
+      <c r="IB846" s="9"/>
+      <c r="IC846" s="9"/>
+      <c r="ID846" s="9"/>
+      <c r="IE846" s="9"/>
+      <c r="IF846" s="9"/>
+      <c r="IG846" s="9"/>
+      <c r="IH846" s="9"/>
+      <c r="II846" s="9"/>
+      <c r="IJ846" s="9"/>
+      <c r="IK846" s="9"/>
+      <c r="IL846" s="9"/>
+      <c r="IM846" s="9"/>
+      <c r="IN846" s="9"/>
+      <c r="IO846" s="9"/>
+      <c r="IP846" s="9"/>
+      <c r="IQ846" s="9"/>
+      <c r="IR846" s="9"/>
+      <c r="IS846" s="9"/>
+      <c r="IT846" s="9"/>
+      <c r="IU846" s="9"/>
+      <c r="IV846" s="9"/>
+      <c r="IW846" s="9"/>
+      <c r="IX846" s="9"/>
+      <c r="IY846" s="9"/>
+      <c r="IZ846" s="9"/>
+      <c r="JA846" s="9"/>
+      <c r="JB846" s="9"/>
+      <c r="JC846" s="9"/>
+      <c r="JD846" s="9"/>
+      <c r="JE846" s="9"/>
+      <c r="JF846" s="9"/>
+      <c r="JG846" s="9"/>
+      <c r="JH846" s="9"/>
+      <c r="JI846" s="9"/>
+      <c r="JJ846" s="9"/>
+      <c r="JK846" s="9"/>
+      <c r="JL846" s="9"/>
+      <c r="JM846" s="9"/>
+      <c r="JN846" s="9"/>
+      <c r="JO846" s="9"/>
+      <c r="JP846" s="9"/>
+      <c r="JQ846" s="9"/>
+      <c r="JR846" s="9"/>
+      <c r="JS846" s="9"/>
+      <c r="JT846" s="9"/>
+      <c r="JU846" s="9"/>
+      <c r="JV846" s="9"/>
+      <c r="JW846" s="9"/>
+      <c r="JX846" s="9"/>
+      <c r="JY846" s="9"/>
+      <c r="JZ846" s="9"/>
+      <c r="KA846" s="9"/>
+      <c r="KB846" s="9"/>
+      <c r="KC846" s="9"/>
+      <c r="KD846" s="9"/>
+      <c r="KE846" s="9"/>
+      <c r="KF846" s="9"/>
+      <c r="KG846" s="9"/>
+      <c r="KH846" s="9"/>
+      <c r="KI846" s="9"/>
+      <c r="KJ846" s="9"/>
+      <c r="KK846" s="9"/>
+      <c r="KL846" s="9"/>
+      <c r="KM846" s="9"/>
+      <c r="KN846" s="9"/>
+      <c r="KO846" s="9"/>
+      <c r="KP846" s="9"/>
+      <c r="KQ846" s="9"/>
+      <c r="KR846" s="9"/>
+      <c r="KS846" s="9"/>
+      <c r="KT846" s="9"/>
+      <c r="KU846" s="9"/>
+      <c r="KV846" s="9"/>
+      <c r="KW846" s="9"/>
+      <c r="KX846" s="9"/>
+      <c r="KY846" s="9"/>
+      <c r="KZ846" s="9"/>
+      <c r="LA846" s="9"/>
+      <c r="LB846" s="9"/>
+      <c r="LC846" s="9"/>
+      <c r="LD846" s="9"/>
+      <c r="LE846" s="9"/>
+      <c r="LF846" s="9"/>
+      <c r="LG846" s="9"/>
+      <c r="LH846" s="9"/>
+      <c r="LI846" s="9"/>
+      <c r="LJ846" s="9"/>
+      <c r="LK846" s="9"/>
+      <c r="LL846" s="9"/>
+      <c r="LM846" s="9"/>
+      <c r="LN846" s="9"/>
+      <c r="LO846" s="9"/>
+      <c r="LP846" s="9"/>
+      <c r="LQ846" s="9"/>
+      <c r="LR846" s="9"/>
+      <c r="LS846" s="9"/>
+      <c r="LT846" s="9"/>
+      <c r="LU846" s="9"/>
+      <c r="LV846" s="9"/>
+      <c r="LW846" s="9"/>
+      <c r="LX846" s="9"/>
+      <c r="LY846" s="9"/>
+      <c r="LZ846" s="9"/>
+      <c r="MA846" s="9"/>
+      <c r="MB846" s="9"/>
+      <c r="MC846" s="9"/>
+      <c r="MD846" s="9"/>
+      <c r="ME846" s="9"/>
+      <c r="MF846" s="9"/>
+      <c r="MG846" s="9"/>
+      <c r="MH846" s="9"/>
+      <c r="MI846" s="9"/>
+      <c r="MJ846" s="9"/>
+      <c r="MK846" s="9"/>
+      <c r="ML846" s="9"/>
+      <c r="MM846" s="9"/>
+      <c r="MN846" s="9"/>
+      <c r="MO846" s="9"/>
+      <c r="MP846" s="9"/>
+      <c r="MQ846" s="9"/>
+      <c r="MR846" s="9"/>
+      <c r="MS846" s="9"/>
+      <c r="MT846" s="9"/>
+      <c r="MU846" s="9"/>
+      <c r="MV846" s="9"/>
+      <c r="MW846" s="9"/>
+      <c r="MX846" s="9"/>
+      <c r="MY846" s="9"/>
+      <c r="MZ846" s="9"/>
+      <c r="NA846" s="9"/>
+      <c r="NB846" s="9"/>
+      <c r="NC846" s="9"/>
+      <c r="ND846" s="9"/>
+      <c r="NE846" s="9"/>
+      <c r="NF846" s="9"/>
+      <c r="NG846" s="9"/>
+      <c r="NH846" s="9"/>
+      <c r="NI846" s="9"/>
+      <c r="NJ846" s="9"/>
+      <c r="NK846" s="9"/>
+      <c r="NL846" s="9"/>
+      <c r="NM846" s="9"/>
+      <c r="NN846" s="9"/>
+      <c r="NO846" s="9"/>
+      <c r="NP846" s="9"/>
+      <c r="NQ846" s="9"/>
+      <c r="NR846" s="9"/>
+      <c r="NS846" s="9"/>
+      <c r="NT846" s="9"/>
+      <c r="NU846" s="9"/>
+      <c r="NV846" s="9"/>
+      <c r="NW846" s="9"/>
+      <c r="NX846" s="9"/>
+      <c r="NY846" s="9"/>
+      <c r="NZ846" s="9"/>
+      <c r="OA846" s="9"/>
+      <c r="OB846" s="9"/>
+      <c r="OC846" s="9"/>
+      <c r="OD846" s="9"/>
+      <c r="OE846" s="9"/>
+      <c r="OF846" s="9"/>
+      <c r="OG846" s="9"/>
+      <c r="OH846" s="9"/>
+      <c r="OI846" s="9"/>
+      <c r="OJ846" s="9"/>
+      <c r="OK846" s="9"/>
+      <c r="OL846" s="9"/>
+      <c r="OM846" s="9"/>
+      <c r="ON846" s="9"/>
+      <c r="OO846" s="9"/>
+      <c r="OP846" s="9"/>
+      <c r="OQ846" s="9"/>
+      <c r="OR846" s="9"/>
+      <c r="OS846" s="9"/>
+      <c r="OT846" s="9"/>
+      <c r="OU846" s="9"/>
+      <c r="OV846" s="9"/>
+      <c r="OW846" s="9"/>
+      <c r="OX846" s="9"/>
+      <c r="OY846" s="9"/>
+      <c r="OZ846" s="9"/>
+      <c r="PA846" s="9"/>
+      <c r="PB846" s="9"/>
+      <c r="PC846" s="9"/>
+      <c r="PD846" s="9"/>
+      <c r="PE846" s="9"/>
+      <c r="PF846" s="9"/>
+      <c r="PG846" s="9"/>
+      <c r="PH846" s="9"/>
+      <c r="PI846" s="9"/>
+      <c r="PJ846" s="9"/>
+      <c r="PK846" s="9"/>
+      <c r="PL846" s="9"/>
+      <c r="PM846" s="9"/>
+      <c r="PN846" s="9"/>
+      <c r="PO846" s="9"/>
+      <c r="PP846" s="9"/>
+      <c r="PQ846" s="9"/>
+      <c r="PR846" s="9"/>
+      <c r="PS846" s="9"/>
+      <c r="PT846" s="9"/>
+      <c r="PU846" s="9"/>
+      <c r="PV846" s="9"/>
+      <c r="PW846" s="9"/>
+      <c r="PX846" s="9"/>
+      <c r="PY846" s="9"/>
+      <c r="PZ846" s="9"/>
+      <c r="QA846" s="9"/>
+      <c r="QB846" s="9"/>
+      <c r="QC846" s="9"/>
+      <c r="QD846" s="9"/>
+      <c r="QE846" s="9"/>
+      <c r="QF846" s="9"/>
+      <c r="QG846" s="9"/>
+      <c r="QH846" s="9"/>
+      <c r="QI846" s="9"/>
+      <c r="QJ846" s="9"/>
+      <c r="QK846" s="9"/>
+      <c r="QL846" s="9"/>
+      <c r="QM846" s="9"/>
+      <c r="QN846" s="9"/>
+      <c r="QO846" s="9"/>
+      <c r="QP846" s="9"/>
+      <c r="QQ846" s="9"/>
+      <c r="QR846" s="9"/>
+      <c r="QS846" s="9"/>
+      <c r="QT846" s="9"/>
+      <c r="QU846" s="9"/>
+      <c r="QV846" s="9"/>
+      <c r="QW846" s="9"/>
+      <c r="QX846" s="9"/>
+      <c r="QY846" s="9"/>
+      <c r="QZ846" s="9"/>
+      <c r="RA846" s="9"/>
+      <c r="RB846" s="9"/>
+      <c r="RC846" s="9"/>
+      <c r="RD846" s="9"/>
+      <c r="RE846" s="9"/>
+      <c r="RF846" s="9"/>
+      <c r="RG846" s="9"/>
+      <c r="RH846" s="9"/>
+      <c r="RI846" s="9"/>
+      <c r="RJ846" s="9"/>
+      <c r="RK846" s="9"/>
+      <c r="RL846" s="9"/>
+      <c r="RM846" s="9"/>
+      <c r="RN846" s="9"/>
+      <c r="RO846" s="9"/>
+      <c r="RP846" s="9"/>
+      <c r="RQ846" s="9"/>
+      <c r="RR846" s="9"/>
+      <c r="RS846" s="9"/>
+      <c r="RT846" s="9"/>
+      <c r="RU846" s="9"/>
+      <c r="RV846" s="9"/>
+      <c r="RW846" s="9"/>
+      <c r="RX846" s="9"/>
+      <c r="RY846" s="9"/>
+      <c r="RZ846" s="9"/>
+      <c r="SA846" s="9"/>
+      <c r="SB846" s="9"/>
+      <c r="SC846" s="9"/>
+      <c r="SD846" s="9"/>
+      <c r="SE846" s="9"/>
+      <c r="SF846" s="9"/>
+      <c r="SG846" s="9"/>
+      <c r="SH846" s="9"/>
+      <c r="SI846" s="9"/>
+      <c r="SJ846" s="9"/>
+      <c r="SK846" s="9"/>
+      <c r="SL846" s="9"/>
+      <c r="SM846" s="9"/>
+      <c r="SN846" s="9"/>
+      <c r="SO846" s="9"/>
+      <c r="SP846" s="9"/>
+      <c r="SQ846" s="9"/>
+      <c r="SR846" s="9"/>
+      <c r="SS846" s="9"/>
+      <c r="ST846" s="9"/>
+      <c r="SU846" s="9"/>
+      <c r="SV846" s="9"/>
+      <c r="SW846" s="9"/>
+      <c r="SX846" s="9"/>
+      <c r="SY846" s="9"/>
+      <c r="SZ846" s="9"/>
+      <c r="TA846" s="9"/>
+      <c r="TB846" s="9"/>
+      <c r="TC846" s="9"/>
+      <c r="TD846" s="9"/>
+      <c r="TE846" s="9"/>
+      <c r="TF846" s="9"/>
+      <c r="TG846" s="9"/>
+      <c r="TH846" s="9"/>
+      <c r="TI846" s="9"/>
+      <c r="TJ846" s="9"/>
+      <c r="TK846" s="9"/>
+      <c r="TL846" s="9"/>
+      <c r="TM846" s="9"/>
+      <c r="TN846" s="9"/>
+      <c r="TO846" s="9"/>
+      <c r="TP846" s="9"/>
+      <c r="TQ846" s="9"/>
+      <c r="TR846" s="9"/>
+      <c r="TS846" s="9"/>
+      <c r="TT846" s="9"/>
+      <c r="TU846" s="9"/>
+      <c r="TV846" s="9"/>
+      <c r="TW846" s="9"/>
+      <c r="TX846" s="9"/>
+      <c r="TY846" s="9"/>
+      <c r="TZ846" s="9"/>
+      <c r="UA846" s="9"/>
+      <c r="UB846" s="9"/>
+      <c r="UC846" s="9"/>
+      <c r="UD846" s="9"/>
+      <c r="UE846" s="9"/>
+      <c r="UF846" s="9"/>
+      <c r="UG846" s="9"/>
+      <c r="UH846" s="9"/>
+      <c r="UI846" s="9"/>
+      <c r="UJ846" s="9"/>
+      <c r="UK846" s="9"/>
+      <c r="UL846" s="9"/>
+      <c r="UM846" s="9"/>
+      <c r="UN846" s="9"/>
+      <c r="UO846" s="9"/>
+      <c r="UP846" s="9"/>
+      <c r="UQ846" s="9"/>
+      <c r="UR846" s="9"/>
+      <c r="US846" s="9"/>
+      <c r="UT846" s="9"/>
+      <c r="UU846" s="9"/>
+      <c r="UV846" s="9"/>
+      <c r="UW846" s="9"/>
+      <c r="UX846" s="9"/>
+      <c r="UY846" s="9"/>
+      <c r="UZ846" s="9"/>
+      <c r="VA846" s="9"/>
+      <c r="VB846" s="9"/>
+      <c r="VC846" s="9"/>
+      <c r="VD846" s="9"/>
+      <c r="VE846" s="9"/>
+      <c r="VF846" s="9"/>
+      <c r="VG846" s="9"/>
+      <c r="VH846" s="9"/>
+      <c r="VI846" s="9"/>
+      <c r="VJ846" s="9"/>
+      <c r="VK846" s="9"/>
+      <c r="VL846" s="9"/>
+      <c r="VM846" s="9"/>
+      <c r="VN846" s="9"/>
+      <c r="VO846" s="9"/>
+      <c r="VP846" s="9"/>
+      <c r="VQ846" s="9"/>
+      <c r="VR846" s="9"/>
+      <c r="VS846" s="9"/>
+      <c r="VT846" s="9"/>
+      <c r="VU846" s="9"/>
+      <c r="VV846" s="9"/>
+      <c r="VW846" s="9"/>
+      <c r="VX846" s="9"/>
+      <c r="VY846" s="9"/>
+      <c r="VZ846" s="9"/>
+      <c r="WA846" s="9"/>
+      <c r="WB846" s="9"/>
+      <c r="WC846" s="9"/>
+      <c r="WD846" s="9"/>
+      <c r="WE846" s="9"/>
+      <c r="WF846" s="9"/>
+      <c r="WG846" s="9"/>
+      <c r="WH846" s="9"/>
+      <c r="WI846" s="9"/>
+      <c r="WJ846" s="9"/>
+      <c r="WK846" s="9"/>
+      <c r="WL846" s="9"/>
+      <c r="WM846" s="9"/>
+      <c r="WN846" s="9"/>
+      <c r="WO846" s="9"/>
+      <c r="WP846" s="9"/>
+      <c r="WQ846" s="9"/>
+      <c r="WR846" s="9"/>
+      <c r="WS846" s="9"/>
+      <c r="WT846" s="9"/>
+      <c r="WU846" s="9"/>
+      <c r="WV846" s="9"/>
+      <c r="WW846" s="9"/>
+      <c r="WX846" s="9"/>
+      <c r="WY846" s="9"/>
+      <c r="WZ846" s="9"/>
+      <c r="XA846" s="9"/>
+      <c r="XB846" s="9"/>
+      <c r="XC846" s="9"/>
+      <c r="XD846" s="9"/>
+      <c r="XE846" s="9"/>
+      <c r="XF846" s="9"/>
+      <c r="XG846" s="9"/>
+      <c r="XH846" s="9"/>
+      <c r="XI846" s="9"/>
+      <c r="XJ846" s="9"/>
+      <c r="XK846" s="9"/>
+      <c r="XL846" s="9"/>
+      <c r="XM846" s="9"/>
+      <c r="XN846" s="9"/>
+      <c r="XO846" s="9"/>
+      <c r="XP846" s="9"/>
+      <c r="XQ846" s="9"/>
+      <c r="XR846" s="9"/>
+      <c r="XS846" s="9"/>
+      <c r="XT846" s="9"/>
+      <c r="XU846" s="9"/>
+      <c r="XV846" s="9"/>
+      <c r="XW846" s="9"/>
+      <c r="XX846" s="9"/>
+      <c r="XY846" s="9"/>
+      <c r="XZ846" s="9"/>
+      <c r="YA846" s="9"/>
+      <c r="YB846" s="9"/>
+      <c r="YC846" s="9"/>
+      <c r="YD846" s="9"/>
+      <c r="YE846" s="9"/>
+      <c r="YF846" s="9"/>
+      <c r="YG846" s="9"/>
+      <c r="YH846" s="9"/>
+      <c r="YI846" s="9"/>
+      <c r="YJ846" s="9"/>
+      <c r="YK846" s="9"/>
+      <c r="YL846" s="9"/>
+      <c r="YM846" s="9"/>
+      <c r="YN846" s="9"/>
+      <c r="YO846" s="9"/>
+      <c r="YP846" s="9"/>
+      <c r="YQ846" s="9"/>
+      <c r="YR846" s="9"/>
+      <c r="YS846" s="9"/>
+      <c r="YT846" s="9"/>
+      <c r="YU846" s="9"/>
+      <c r="YV846" s="9"/>
+      <c r="YW846" s="9"/>
+      <c r="YX846" s="9"/>
+      <c r="YY846" s="9"/>
+      <c r="YZ846" s="9"/>
+      <c r="ZA846" s="9"/>
+      <c r="ZB846" s="9"/>
+      <c r="ZC846" s="9"/>
+      <c r="ZD846" s="9"/>
+      <c r="ZE846" s="9"/>
+      <c r="ZF846" s="9"/>
+      <c r="ZG846" s="9"/>
+      <c r="ZH846" s="9"/>
+      <c r="ZI846" s="9"/>
+      <c r="ZJ846" s="9"/>
+      <c r="ZK846" s="9"/>
+      <c r="ZL846" s="9"/>
+      <c r="ZM846" s="9"/>
+      <c r="ZN846" s="9"/>
+      <c r="ZO846" s="9"/>
+      <c r="ZP846" s="9"/>
+      <c r="ZQ846" s="9"/>
+      <c r="ZR846" s="9"/>
+      <c r="ZS846" s="9"/>
+      <c r="ZT846" s="9"/>
+      <c r="ZU846" s="9"/>
+      <c r="ZV846" s="9"/>
+      <c r="ZW846" s="9"/>
+      <c r="ZX846" s="9"/>
+      <c r="ZY846" s="9"/>
+      <c r="ZZ846" s="9"/>
+      <c r="AAA846" s="9"/>
+      <c r="AAB846" s="9"/>
+      <c r="AAC846" s="9"/>
+      <c r="AAD846" s="9"/>
+      <c r="AAE846" s="9"/>
+      <c r="AAF846" s="9"/>
+      <c r="AAG846" s="9"/>
+      <c r="AAH846" s="9"/>
+      <c r="AAI846" s="9"/>
+      <c r="AAJ846" s="9"/>
+      <c r="AAK846" s="9"/>
+      <c r="AAL846" s="9"/>
+      <c r="AAM846" s="9"/>
+      <c r="AAN846" s="9"/>
+      <c r="AAO846" s="9"/>
+      <c r="AAP846" s="9"/>
+      <c r="AAQ846" s="9"/>
+      <c r="AAR846" s="9"/>
+      <c r="AAS846" s="9"/>
+      <c r="AAT846" s="9"/>
+      <c r="AAU846" s="9"/>
+      <c r="AAV846" s="9"/>
+      <c r="AAW846" s="9"/>
+      <c r="AAX846" s="9"/>
+      <c r="AAY846" s="9"/>
+      <c r="AAZ846" s="9"/>
+      <c r="ABA846" s="9"/>
+      <c r="ABB846" s="9"/>
+      <c r="ABC846" s="9"/>
+      <c r="ABD846" s="9"/>
+      <c r="ABE846" s="9"/>
+      <c r="ABF846" s="9"/>
+      <c r="ABG846" s="9"/>
+      <c r="ABH846" s="9"/>
+      <c r="ABI846" s="9"/>
+      <c r="ABJ846" s="9"/>
+      <c r="ABK846" s="9"/>
+      <c r="ABL846" s="9"/>
+      <c r="ABM846" s="9"/>
+      <c r="ABN846" s="9"/>
+      <c r="ABO846" s="9"/>
+      <c r="ABP846" s="9"/>
+      <c r="ABQ846" s="9"/>
+      <c r="ABR846" s="9"/>
+      <c r="ABS846" s="9"/>
+      <c r="ABT846" s="9"/>
+      <c r="ABU846" s="9"/>
+      <c r="ABV846" s="9"/>
+      <c r="ABW846" s="9"/>
+      <c r="ABX846" s="9"/>
+      <c r="ABY846" s="9"/>
+      <c r="ABZ846" s="9"/>
+      <c r="ACA846" s="9"/>
+      <c r="ACB846" s="9"/>
+      <c r="ACC846" s="9"/>
+      <c r="ACD846" s="9"/>
+      <c r="ACE846" s="9"/>
+      <c r="ACF846" s="9"/>
+      <c r="ACG846" s="9"/>
+      <c r="ACH846" s="9"/>
+      <c r="ACI846" s="9"/>
+      <c r="ACJ846" s="9"/>
+      <c r="ACK846" s="9"/>
+      <c r="ACL846" s="9"/>
+      <c r="ACM846" s="9"/>
+      <c r="ACN846" s="9"/>
+      <c r="ACO846" s="9"/>
+      <c r="ACP846" s="9"/>
+      <c r="ACQ846" s="9"/>
+      <c r="ACR846" s="9"/>
+      <c r="ACS846" s="9"/>
+      <c r="ACT846" s="9"/>
+      <c r="ACU846" s="9"/>
+      <c r="ACV846" s="9"/>
+      <c r="ACW846" s="9"/>
+      <c r="ACX846" s="9"/>
+      <c r="ACY846" s="9"/>
+      <c r="ACZ846" s="9"/>
+      <c r="ADA846" s="9"/>
+      <c r="ADB846" s="9"/>
+      <c r="ADC846" s="9"/>
+      <c r="ADD846" s="9"/>
+      <c r="ADE846" s="9"/>
+      <c r="ADF846" s="9"/>
+      <c r="ADG846" s="9"/>
+      <c r="ADH846" s="9"/>
+      <c r="ADI846" s="9"/>
+      <c r="ADJ846" s="9"/>
+      <c r="ADK846" s="9"/>
+      <c r="ADL846" s="9"/>
+      <c r="ADM846" s="9"/>
+      <c r="ADN846" s="9"/>
+      <c r="ADO846" s="9"/>
+      <c r="ADP846" s="9"/>
+      <c r="ADQ846" s="9"/>
+      <c r="ADR846" s="9"/>
+      <c r="ADS846" s="9"/>
+      <c r="ADT846" s="9"/>
+      <c r="ADU846" s="9"/>
+      <c r="ADV846" s="9"/>
+      <c r="ADW846" s="9"/>
+      <c r="ADX846" s="9"/>
+      <c r="ADY846" s="9"/>
+      <c r="ADZ846" s="9"/>
+      <c r="AEA846" s="9"/>
+      <c r="AEB846" s="9"/>
+      <c r="AEC846" s="9"/>
+      <c r="AED846" s="9"/>
+      <c r="AEE846" s="9"/>
+      <c r="AEF846" s="9"/>
+      <c r="AEG846" s="9"/>
+      <c r="AEH846" s="9"/>
+      <c r="AEI846" s="9"/>
+      <c r="AEJ846" s="9"/>
+      <c r="AEK846" s="9"/>
+      <c r="AEL846" s="9"/>
+      <c r="AEM846" s="9"/>
+      <c r="AEN846" s="9"/>
+      <c r="AEO846" s="9"/>
+      <c r="AEP846" s="9"/>
+      <c r="AEQ846" s="9"/>
+      <c r="AER846" s="9"/>
+      <c r="AES846" s="9"/>
+      <c r="AET846" s="9"/>
+      <c r="AEU846" s="9"/>
+      <c r="AEV846" s="9"/>
+      <c r="AEW846" s="9"/>
+      <c r="AEX846" s="9"/>
+      <c r="AEY846" s="9"/>
+      <c r="AEZ846" s="9"/>
+      <c r="AFA846" s="9"/>
+      <c r="AFB846" s="9"/>
+      <c r="AFC846" s="9"/>
+      <c r="AFD846" s="9"/>
+      <c r="AFE846" s="9"/>
+      <c r="AFF846" s="9"/>
+      <c r="AFG846" s="9"/>
+      <c r="AFH846" s="9"/>
+      <c r="AFI846" s="9"/>
+      <c r="AFJ846" s="9"/>
+      <c r="AFK846" s="9"/>
+      <c r="AFL846" s="9"/>
+      <c r="AFM846" s="9"/>
+      <c r="AFN846" s="9"/>
+      <c r="AFO846" s="9"/>
+      <c r="AFP846" s="9"/>
+      <c r="AFQ846" s="9"/>
+      <c r="AFR846" s="9"/>
+      <c r="AFS846" s="9"/>
+      <c r="AFT846" s="9"/>
+      <c r="AFU846" s="9"/>
+      <c r="AFV846" s="9"/>
+      <c r="AFW846" s="9"/>
+      <c r="AFX846" s="9"/>
+      <c r="AFY846" s="9"/>
+      <c r="AFZ846" s="9"/>
+      <c r="AGA846" s="9"/>
+      <c r="AGB846" s="9"/>
+      <c r="AGC846" s="9"/>
+      <c r="AGD846" s="9"/>
+      <c r="AGE846" s="9"/>
+      <c r="AGF846" s="9"/>
+      <c r="AGG846" s="9"/>
+      <c r="AGH846" s="9"/>
+      <c r="AGI846" s="9"/>
+      <c r="AGJ846" s="9"/>
+      <c r="AGK846" s="9"/>
+      <c r="AGL846" s="9"/>
+      <c r="AGM846" s="9"/>
+      <c r="AGN846" s="9"/>
+      <c r="AGO846" s="9"/>
+      <c r="AGP846" s="9"/>
+      <c r="AGQ846" s="9"/>
+      <c r="AGR846" s="9"/>
+      <c r="AGS846" s="9"/>
+      <c r="AGT846" s="9"/>
+      <c r="AGU846" s="9"/>
+      <c r="AGV846" s="9"/>
+      <c r="AGW846" s="9"/>
+      <c r="AGX846" s="9"/>
+      <c r="AGY846" s="9"/>
+      <c r="AGZ846" s="9"/>
+      <c r="AHA846" s="9"/>
+      <c r="AHB846" s="9"/>
+      <c r="AHC846" s="9"/>
+      <c r="AHD846" s="9"/>
+      <c r="AHE846" s="9"/>
+      <c r="AHF846" s="9"/>
+      <c r="AHG846" s="9"/>
+      <c r="AHH846" s="9"/>
+      <c r="AHI846" s="9"/>
+      <c r="AHJ846" s="9"/>
+      <c r="AHK846" s="9"/>
+      <c r="AHL846" s="9"/>
+      <c r="AHM846" s="9"/>
+      <c r="AHN846" s="9"/>
+      <c r="AHO846" s="9"/>
+      <c r="AHP846" s="9"/>
+      <c r="AHQ846" s="9"/>
+      <c r="AHR846" s="9"/>
+      <c r="AHS846" s="9"/>
+      <c r="AHT846" s="9"/>
+      <c r="AHU846" s="9"/>
+      <c r="AHV846" s="9"/>
+      <c r="AHW846" s="9"/>
+      <c r="AHX846" s="9"/>
+      <c r="AHY846" s="9"/>
+      <c r="AHZ846" s="9"/>
+      <c r="AIA846" s="9"/>
+      <c r="AIB846" s="9"/>
+      <c r="AIC846" s="9"/>
+      <c r="AID846" s="9"/>
+      <c r="AIE846" s="9"/>
+      <c r="AIF846" s="9"/>
+      <c r="AIG846" s="9"/>
+      <c r="AIH846" s="9"/>
+      <c r="AII846" s="9"/>
+      <c r="AIJ846" s="9"/>
+      <c r="AIK846" s="9"/>
+      <c r="AIL846" s="9"/>
+      <c r="AIM846" s="9"/>
+      <c r="AIN846" s="9"/>
+      <c r="AIO846" s="9"/>
+      <c r="AIP846" s="9"/>
+      <c r="AIQ846" s="9"/>
+      <c r="AIR846" s="9"/>
+      <c r="AIS846" s="9"/>
+      <c r="AIT846" s="9"/>
+      <c r="AIU846" s="9"/>
+      <c r="AIV846" s="9"/>
+      <c r="AIW846" s="9"/>
+      <c r="AIX846" s="9"/>
+      <c r="AIY846" s="9"/>
+      <c r="AIZ846" s="9"/>
+      <c r="AJA846" s="9"/>
+      <c r="AJB846" s="9"/>
+      <c r="AJC846" s="9"/>
+      <c r="AJD846" s="9"/>
+      <c r="AJE846" s="9"/>
+      <c r="AJF846" s="9"/>
+      <c r="AJG846" s="9"/>
+      <c r="AJH846" s="9"/>
+      <c r="AJI846" s="9"/>
+      <c r="AJJ846" s="9"/>
+      <c r="AJK846" s="9"/>
+      <c r="AJL846" s="9"/>
+      <c r="AJM846" s="9"/>
+      <c r="AJN846" s="9"/>
+      <c r="AJO846" s="9"/>
+      <c r="AJP846" s="9"/>
+      <c r="AJQ846" s="9"/>
+      <c r="AJR846" s="9"/>
+      <c r="AJS846" s="9"/>
+      <c r="AJT846" s="9"/>
+      <c r="AJU846" s="9"/>
+      <c r="AJV846" s="9"/>
+      <c r="AJW846" s="9"/>
+      <c r="AJX846" s="9"/>
+      <c r="AJY846" s="9"/>
+      <c r="AJZ846" s="9"/>
+      <c r="AKA846" s="9"/>
+      <c r="AKB846" s="9"/>
+      <c r="AKC846" s="9"/>
+      <c r="AKD846" s="9"/>
+      <c r="AKE846" s="9"/>
+      <c r="AKF846" s="9"/>
+      <c r="AKG846" s="9"/>
+      <c r="AKH846" s="9"/>
+      <c r="AKI846" s="9"/>
+      <c r="AKJ846" s="9"/>
+      <c r="AKK846" s="9"/>
+      <c r="AKL846" s="9"/>
+      <c r="AKM846" s="9"/>
+      <c r="AKN846" s="9"/>
+      <c r="AKO846" s="9"/>
+      <c r="AKP846" s="9"/>
+      <c r="AKQ846" s="9"/>
+      <c r="AKR846" s="9"/>
+      <c r="AKS846" s="9"/>
+      <c r="AKT846" s="9"/>
+      <c r="AKU846" s="9"/>
+      <c r="AKV846" s="9"/>
+      <c r="AKW846" s="9"/>
+      <c r="AKX846" s="9"/>
+      <c r="AKY846" s="9"/>
+      <c r="AKZ846" s="9"/>
+      <c r="ALA846" s="9"/>
+      <c r="ALB846" s="9"/>
+      <c r="ALC846" s="9"/>
+      <c r="ALD846" s="9"/>
+      <c r="ALE846" s="9"/>
+      <c r="ALF846" s="9"/>
+      <c r="ALG846" s="9"/>
+      <c r="ALH846" s="9"/>
+      <c r="ALI846" s="9"/>
+      <c r="ALJ846" s="9"/>
+      <c r="ALK846" s="9"/>
+      <c r="ALL846" s="9"/>
+      <c r="ALM846" s="9"/>
+      <c r="ALN846" s="9"/>
+      <c r="ALO846" s="9"/>
+      <c r="ALP846" s="9"/>
+      <c r="ALQ846" s="9"/>
+      <c r="ALR846" s="9"/>
+      <c r="ALS846" s="9"/>
+      <c r="ALT846" s="9"/>
+      <c r="ALU846" s="9"/>
+      <c r="ALV846" s="9"/>
+      <c r="ALW846" s="9"/>
+      <c r="ALX846" s="9"/>
+      <c r="ALY846" s="9"/>
+      <c r="ALZ846" s="9"/>
+      <c r="AMA846" s="9"/>
+      <c r="AMB846" s="9"/>
+      <c r="AMC846" s="9"/>
+      <c r="AMD846" s="9"/>
+      <c r="AME846" s="9"/>
+      <c r="AMF846" s="9"/>
+      <c r="AMG846" s="9"/>
+      <c r="AMH846" s="9"/>
+      <c r="AMI846" s="9"/>
+      <c r="AMJ846" s="9"/>
+      <c r="AMK846" s="9"/>
     </row>
     <row r="847" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A847" s="1" t="s">
-        <v>987</v>
-      </c>
-      <c r="AM847" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN847" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO847" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP847" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="AI847" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ847" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="848" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A848" s="1" t="s">
-        <v>988</v>
-      </c>
-      <c r="AI848" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ848" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE848" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF848" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="AM848" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN848" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO848" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP848" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="849" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A849" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="BC849" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD849" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="AI849" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ849" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE849" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF849" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="850" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A850" s="1" t="s">
-        <v>990</v>
-      </c>
-      <c r="AK850" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL850" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="BC850" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD850" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="851" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A851" s="1" t="s">
-        <v>992</v>
-      </c>
-      <c r="AI851" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ851" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU851" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV851" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="AK851" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL851" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="852" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A852" s="1" t="s">
-        <v>993</v>
-      </c>
-      <c r="BA852" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB852" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="AI852" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ852" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU852" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV852" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="853" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A853" s="1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="AA853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ853" s="1" t="s">
-        <v>16</v>
+        <v>993</v>
       </c>
       <c r="BA853" s="1" t="s">
         <v>16</v>
       </c>
       <c r="BB853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG853" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BH853" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="854" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A854" s="1" t="s">
-        <v>991</v>
+        <v>1016</v>
+      </c>
+      <c r="AA854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ854" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="AK854" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AL854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG854" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH854" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="855" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A855" s="1" t="s">
-        <v>994</v>
-      </c>
-      <c r="AA855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ855" s="1" t="s">
-        <v>16</v>
+        <v>991</v>
       </c>
       <c r="AK855" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AL855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BA855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG855" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BH855" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="856" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A856" s="1" t="s">
-        <v>952</v>
-      </c>
-      <c r="U856" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="AA856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG856" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH856" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="857" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A857" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U857" s="1" t="s">
         <v>16</v>
@@ -19077,40 +19077,37 @@
     </row>
     <row r="858" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A858" s="1" t="s">
-        <v>954</v>
-      </c>
-      <c r="P858" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q858" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="U858" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="859" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A859" s="1" t="s">
-        <v>955</v>
-      </c>
-      <c r="R859" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S859" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="P859" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q859" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="860" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A860" s="1" t="s">
-        <v>956</v>
-      </c>
-      <c r="P860" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q860" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="R860" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S860" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="861" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A861" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="P861" s="1" t="s">
         <v>16</v>
@@ -19121,7 +19118,7 @@
     </row>
     <row r="862" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A862" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="P862" s="1" t="s">
         <v>16</v>
@@ -19132,7 +19129,7 @@
     </row>
     <row r="863" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A863" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="P863" s="1" t="s">
         <v>16</v>
@@ -19143,7 +19140,7 @@
     </row>
     <row r="864" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A864" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="P864" s="1" t="s">
         <v>16</v>
@@ -19154,7 +19151,7 @@
     </row>
     <row r="865" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A865" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="P865" s="1" t="s">
         <v>16</v>
@@ -19165,7 +19162,7 @@
     </row>
     <row r="866" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A866" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="P866" s="1" t="s">
         <v>16</v>
@@ -19176,7 +19173,7 @@
     </row>
     <row r="867" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A867" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="P867" s="1" t="s">
         <v>16</v>
@@ -19187,7 +19184,7 @@
     </row>
     <row r="868" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A868" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="P868" s="1" t="s">
         <v>16</v>
@@ -19198,7 +19195,7 @@
     </row>
     <row r="869" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A869" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="P869" s="1" t="s">
         <v>16</v>
@@ -19209,7 +19206,7 @@
     </row>
     <row r="870" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A870" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="P870" s="1" t="s">
         <v>16</v>
@@ -19220,7 +19217,7 @@
     </row>
     <row r="871" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A871" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="P871" s="1" t="s">
         <v>16</v>
@@ -19231,150 +19228,54 @@
     </row>
     <row r="872" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A872" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="P872" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q872" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R872" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S872" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="873" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A873" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="P873" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q873" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R873" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S873" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="874" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A874" s="1" t="s">
-        <v>970</v>
-      </c>
-      <c r="U874" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="P874" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q874" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="875" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A875" s="1" t="s">
-        <v>1017</v>
-      </c>
-      <c r="AA875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BA875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG875" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BH875" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="U875" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="876" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A876" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="AA876" s="1" t="s">
         <v>16</v>
@@ -19481,7 +19382,7 @@
     </row>
     <row r="877" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A877" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="AA877" s="1" t="s">
         <v>16</v>
@@ -19588,7 +19489,7 @@
     </row>
     <row r="878" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A878" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="AA878" s="1" t="s">
         <v>16</v>
@@ -19695,7 +19596,7 @@
     </row>
     <row r="879" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A879" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="AA879" s="1" t="s">
         <v>16</v>
@@ -19802,7 +19703,7 @@
     </row>
     <row r="880" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A880" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="AA880" s="1" t="s">
         <v>16</v>
@@ -19909,113 +19810,220 @@
     </row>
     <row r="881" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A881" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AA881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG881" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH881" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="882" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A882" s="1" t="s">
         <v>1023</v>
       </c>
-      <c r="AA881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AO881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BA881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BF881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG881" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BH881" s="1" t="s">
+      <c r="AA882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG882" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH882" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:BH881">
+  <sortState ref="A2:BH882">
     <sortCondition ref="A41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>